<commit_message>
adding in feedback from coauthors
</commit_message>
<xml_diff>
--- a/Documents/ODMAP-Table.xlsx
+++ b/Documents/ODMAP-Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarahhart/Library/CloudStorage/GoogleDrive-sarahjanehart13@gmail.com/My Drive/JOB/RESEARCH/Analyses/AspenHabitat/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBBCE07E-4A12-E24A-8C6C-1C115CC54D49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B82CDB80-30D2-0B47-ADCD-23624A19EF90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35560" yWindow="-6020" windowWidth="15480" windowHeight="18740" xr2:uid="{13C9FE07-A4C9-0B4A-BF1F-85133AC3EB69}"/>
+    <workbookView xWindow="0" yWindow="3680" windowWidth="38400" windowHeight="17920" xr2:uid="{13C9FE07-A4C9-0B4A-BF1F-85133AC3EB69}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -89,12 +89,6 @@
     <t>Scale of analysis</t>
   </si>
   <si>
-    <t>Title:</t>
-  </si>
-  <si>
-    <t>DOI:</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -168,6 +162,9 @@
     <t>Software</t>
   </si>
   <si>
+    <t>Data</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -176,20 +173,41 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>Data availability</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>: Data are available from XXXX</t>
-    </r>
-  </si>
-  <si>
-    <t>Data</t>
+      <t>Taxon names</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>: Trembling aspen (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Populus tremuloides)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Taxonomic reference system: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>US Department of Agriculture (USDA) Plant List of Attributes, Names, Taxonomy, and Symbols (PLANTS) Database</t>
+    </r>
   </si>
   <si>
     <r>
@@ -200,40 +218,16 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>Taxon names</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>: Trembling aspen (</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Populus tremuloides)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Taxonomic reference system: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>US Department of Agriculture (USDA) Plant List of Attributes, Names, Taxonomy, and Symbols (PLANTS) Database</t>
+      <t>Ecological level</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>: population</t>
     </r>
   </si>
   <si>
@@ -245,17 +239,48 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>Ecological level</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>: population</t>
-    </r>
+      <t xml:space="preserve">Ecoregion mask: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>We clipped all data to the Southern Rocky Mountain Ecoregion using data from the EPA's (2013) Level III Ecoregions of the Conterminous United States product.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Sample size: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">The aspen dataset consists of 4,312,302,640 10 x 10 m cells, of which 117,140,964 recorded the presence of aspen. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Scaling</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>: We aggregated the aspen presence-absence data to a 90 x 90 m cell size.</t>
+    </r>
+  </si>
+  <si>
+    <t>Data partitioning</t>
   </si>
   <si>
     <r>
@@ -266,48 +291,17 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve">Ecoregion mask: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>We clipped all data to the Southern Rocky Mountain Ecoregion using data from the EPA's (2013) Level III Ecoregions of the Conterminous United States product.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Sample size: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">The aspen dataset consists of 4,312,302,640 10 x 10 m cells, of which 117,140,964 recorded the presence of aspen. </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Scaling</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>: We aggregated the aspen presence-absence data to a 90 x 90 m cell size.</t>
-    </r>
-  </si>
-  <si>
-    <t>Data partitioning</t>
+      <t>Contact email:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> sarah.hart@colostate.edu</t>
+    </r>
   </si>
   <si>
     <r>
@@ -318,27 +312,6 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>Contact email:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> sarah.hart@colostate.edu</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
       <t>Spatial resolution</t>
     </r>
     <r>
@@ -349,27 +322,6 @@
         <family val="1"/>
       </rPr>
       <t>: 90 x 90 m</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Code availability</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>: All code is publicly available on GitHub (LINK)</t>
     </r>
   </si>
   <si>
@@ -607,34 +559,6 @@
   </si>
   <si>
     <r>
-      <t>Data source</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>: Aspen presence-absence data at 10x10 m spatial resolution were obtained from Cook et al. (in review).</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Absence data: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>The Cook et al. (in review) map consists of both presence and absence data.</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>Sampling design</t>
     </r>
     <r>
@@ -1110,13 +1034,7 @@
     </r>
   </si>
   <si>
-    <t>To avoid collinearity between climate predictors, we initially screened the 34 climatic variables at their original resolution (i.e. 1 x 1 km). To this end, we calculated pairwise correlation coefficients and when |r|&gt;0.75, we removed variables based on existing research (Table 4). Where evidence was similar, we used univariate random forest (RF) models to evaluate the potential explanatory power of each predictor.</t>
-  </si>
-  <si>
     <t>Using the downscaled climate variables in combination with soil and topographic variables, we further reduced multicollinearity in our predictor dataset by calculating variable inflation factors (VIF) using the spatialRF package (Benito 2022). We then iteratively removed variables until VIF&lt;5 for all variables.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Using the R package DALEX (Biecek 2018), we determined variable importance using a model-agnostic permutation-based approach. In this approach, each variable is randomized and then AUC statistic is compared with =AUC for the full model (where data has not been randomized). We evaluated the relationship between aspen presence and each predictor variable using accumulated local effects (ALE) profiles, which were generated using the ALEPlot package (Aplet, 2018). </t>
   </si>
   <si>
     <t xml:space="preserve">We calculated a weighted probability of occurrence from all four SDMs. Weights assigned were based on the AUC statistic. </t>
@@ -1185,6 +1103,99 @@
       </rPr>
       <t>: Sarah J. Hart, Asha Paudel, and Maxwell C. Cook</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">DOI: </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Title: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Climate-driven decreases in aspen's distribution and opportunities for future expansion across the Southern Rocky Mountains</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Code availability</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Data availability</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Data source</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>: Aspen presence-absence data at 10x10 m spatial resolution were obtained from Cook et al. (2024).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Absence data: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>The Cook et al. (2024) map consists of both presence and absence data.</t>
+    </r>
+  </si>
+  <si>
+    <t>To avoid collinearity between climate predictors, we initially screened the 34 climatic variables at their original resolution (i.e. 1 x 1 km). To this end, we calculated pairwise correlation coefficients and when |r|&gt;0.75, we removed variables based on existing research (Table 5). Where evidence was similar, we used univariate random forest (RF) models to evaluate the potential explanatory power of each predictor.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Using the R package DALEX (Biecek 2018), we determined variable importance using a model-agnostic permutation-based approach. In this approach, each variable is randomized and then AUC statistic is compared with the AUC for the full model (where data has not been randomized). We evaluated the relationship between aspen presence and each predictor variable using accumulated local effects (ALE) profiles, which were generated using the ALEPlot package (Aplet, 2018). </t>
   </si>
 </sst>
 </file>
@@ -1292,7 +1303,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1336,26 +1347,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1673,8 +1675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A126CE3-F8D1-E044-856E-7390C8836DBA}">
   <dimension ref="A1:B58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1693,47 +1695,47 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="15"/>
+      <c r="B2" s="17"/>
     </row>
     <row r="3" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="15" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="17"/>
+      <c r="A4" s="15"/>
       <c r="B4" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="17"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="15"/>
       <c r="B5" s="8" t="s">
-        <v>10</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="18"/>
+      <c r="A6" s="16"/>
       <c r="B6" s="9" t="s">
-        <v>11</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="18" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="18"/>
+      <c r="A8" s="16"/>
       <c r="B8" s="11" t="s">
         <v>5</v>
       </c>
@@ -1743,7 +1745,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -1755,339 +1757,344 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="18" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="17"/>
+      <c r="A12" s="15"/>
       <c r="B12" s="7" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A13" s="17"/>
-      <c r="B13" s="19" t="s">
-        <v>83</v>
+      <c r="A13" s="15"/>
+      <c r="B13" s="7" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="18"/>
+      <c r="A14" s="16"/>
       <c r="B14" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="16" t="s">
+    <row r="16" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="16"/>
+      <c r="B16" s="9" t="s">
         <v>13</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="18"/>
-      <c r="B16" s="9" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="136" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="20" t="s">
-        <v>82</v>
+        <v>17</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A20" s="16" t="s">
-        <v>20</v>
+      <c r="A20" s="18" t="s">
+        <v>18</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A21" s="17"/>
+      <c r="A21" s="15"/>
       <c r="B21" s="8" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="18"/>
+      <c r="A22" s="16"/>
       <c r="B22" s="9" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="68" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A24" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="15"/>
+      <c r="B25" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="16"/>
+      <c r="B26" s="11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A24" s="17" t="s">
+      <c r="B27" s="17"/>
+    </row>
+    <row r="28" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" s="17"/>
-      <c r="B25" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="18"/>
-      <c r="B26" s="21" t="s">
+    </row>
+    <row r="29" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A29" s="15"/>
+      <c r="B29" s="14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="15" t="s">
+    <row r="30" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="15"/>
+      <c r="B30" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B27" s="15"/>
-    </row>
-    <row r="28" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="B28" s="11" t="s">
+    </row>
+    <row r="31" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A31" s="15"/>
+      <c r="B31" s="14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A32" s="15"/>
+      <c r="B32" s="14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A33" s="15"/>
+      <c r="B33" s="14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A34" s="15"/>
+      <c r="B34" s="12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A29" s="17"/>
-      <c r="B29" s="14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="17"/>
-      <c r="B30" s="12" t="s">
+    <row r="35" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A35" s="15"/>
+      <c r="B35" s="14" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A31" s="17"/>
-      <c r="B31" s="14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A32" s="17"/>
-      <c r="B32" s="14" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A33" s="17"/>
-      <c r="B33" s="14" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A34" s="17"/>
-      <c r="B34" s="12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A35" s="17"/>
-      <c r="B35" s="14" t="s">
-        <v>30</v>
-      </c>
-    </row>
     <row r="36" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A36" s="17"/>
+      <c r="A36" s="15"/>
       <c r="B36" s="12" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A37" s="18"/>
+      <c r="A37" s="16"/>
       <c r="B37" s="14" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="85" x14ac:dyDescent="0.2">
-      <c r="A39" s="16" t="s">
-        <v>71</v>
+      <c r="A39" s="18" t="s">
+        <v>65</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A40" s="17"/>
+      <c r="A40" s="15"/>
       <c r="B40" s="12" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="85" x14ac:dyDescent="0.2">
-      <c r="A41" s="17"/>
+      <c r="A41" s="15"/>
       <c r="B41" s="12" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="102" x14ac:dyDescent="0.2">
-      <c r="A42" s="17"/>
+      <c r="A42" s="15"/>
       <c r="B42" s="12" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A43" s="17"/>
+      <c r="A43" s="15"/>
       <c r="B43" s="12" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="204" x14ac:dyDescent="0.2">
-      <c r="A44" s="18"/>
+      <c r="A44" s="16"/>
       <c r="B44" s="12" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="B45" s="15"/>
+      <c r="A45" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B45" s="17"/>
     </row>
     <row r="46" spans="1:2" ht="102" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="68" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="408" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="102" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="B53" s="15"/>
+      <c r="A53" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B53" s="17"/>
     </row>
     <row r="54" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="B56" s="15"/>
+      <c r="A56" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B56" s="17"/>
     </row>
     <row r="57" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="102" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A39:A44"/>
+    <mergeCell ref="A28:A37"/>
     <mergeCell ref="A24:A26"/>
     <mergeCell ref="A53:B53"/>
     <mergeCell ref="A2:B2"/>
@@ -2096,11 +2103,6 @@
     <mergeCell ref="A11:A14"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="A20:A22"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A39:A44"/>
-    <mergeCell ref="A28:A37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>